<commit_message>
Revert "New Russian Localisation"
</commit_message>
<xml_diff>
--- a/CustomLocalization/Localization/RogueTech/RU/Argo Upg/LocalizationDef.xlsx
+++ b/CustomLocalization/Localization/RogueTech/RU/Argo Upg/LocalizationDef.xlsx
@@ -76,14 +76,14 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;b&gt;&lt;color=#F79232&gt;Enables to Drop 1 additional Mech or Tank.&lt;/color&gt;&lt;/b&gt; 
-  So it turns out the docking cradles were salvaged for parts and scrap, but the mounting points are still intact. I can get my techs to work fabricating new 'Mech cradles commander, but it's gonna take a while to get everything rebuilt. I think there's enough pieces left behind to get one assembled quickly, though.
+So it turns out the docking cradles were salvaged for parts and scrap, but the mounting points are still intact. I can get my techs to work fabricating new 'Mech cradles commander, but it's gonna take a while to get everything rebuilt. I think there's enough pieces left behind to get one assembled quickly, though.
 ---
 &lt;b&gt;&lt;color=#F79232&gt;Enables to Drop 1 additional Mech or Tank.&lt;/color&gt;&lt;/b&gt; 
  So it turns out the docking cradles were salvaged for parts and scrap, but the mounting points are still intact. I can get my techs to work fabricating new 'Mech cradles commander, but it's gonna take a while to get everything rebuilt. I think there's enough pieces left behind to get one assembled quickly, though.</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;b&gt;&lt;color=#F79232&gt;Позволяет высадить 1 дополнительный мех или танк.&lt;/color&gt;&lt;/b&gt; 
-  Похоже, что док-станции были разобраны на запчасти, но места крепления остались невредимы. Я могу попросить моих техов поработать над изготовлением новых док-станций для мехов, командир, но потребуется время, чтобы всё воссоздать заново. Хотя, думаю, тут валяется достаточно частей, чтобы быстро собрать хотя бы одну из них.</t>
+Похоже, что док-станции были разобраны на запчасти, но места крепления остались невредимы. Я могу попросить моих техов поработать над изготовлением новых док-станций для мехов, командир, но потребуется время, чтобы всё воссоздать заново. Хотя, думаю, тут валяется достаточно частей, чтобы быстро собрать хотя бы одну из них.</t>
   </si>
   <si>
     <t>argoUpgrade_DropSlot.Description.Name</t>
@@ -99,14 +99,14 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;b&gt;&lt;color=#F79232&gt;Enables to Drop 1 additional Mech or Tank.&lt;/color&gt;&lt;/b&gt; 
-  The first cradle turned out alright, Boss. There's enough scrap left lying around we should be able to construct the bones of a gantry for the next, but we're also gonna need to buy several complex components to get the next cradle ready for use.
+The first cradle turned out alright, Boss. There's enough scrap left lying around we should be able to construct the bones of a gantry for the next, but we're also gonna need to buy several complex components to get the next cradle ready for use.
 ---
 &lt;b&gt;&lt;color=#F79232&gt;Enables to Drop 1 additional Mech or Tank.&lt;/color&gt;&lt;/b&gt; 
  The first cradle turned out alright, Boss. There's enough scrap left lying around we should be able to construct the bones of a gantry for the next, but we're also gonna need to buy several complex components to get the next cradle ready for use.</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;b&gt;&lt;color=#F79232&gt;Позволяет высадить 1 дополнительный мех или танк.&lt;/color&gt;&lt;/b&gt; 
-  Первая док-станция в порядке, босс. Вокруг осталось достаточно металлолома, чтобы мы могли соорудить каркас для ещё одной, но нам точно нужно закупить ещё несколько сложных компонентов, чтобы подготовить док-станцию к использованию.</t>
+Первая док-станция в порядке, босс. Вокруг осталось достаточно металлолома, чтобы мы могли соорудить каркас для ещё одной, но нам точно нужно закупить ещё несколько сложных компонентов, чтобы подготовить док-станцию к использованию.</t>
   </si>
   <si>
     <t>argoUpgrade_DropSlot1.Description.Name</t>
@@ -116,14 +116,14 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;b&gt;&lt;color=#F79232&gt;Enables to Drop 1 additional Mech or Tank.&lt;/color&gt;&lt;/b&gt; 
-  Half-done now, Boss. It's really starting to look like a proper dropship. I can get started on fabricating parts to assemble the final 2 cradles from scratch. Producing the parts in duplicate should save us a little time and money.
+Half-done now, Boss. It's really starting to look like a proper dropship. I can get started on fabricating parts to assemble the final 2 cradles from scratch. Producing the parts in duplicate should save us a little time and money.
 ---
 &lt;b&gt;&lt;color=#F79232&gt;Enables to Drop 1 additional Mech or Tank.&lt;/color&gt;&lt;/b&gt; 
  Half-done now, Boss. It's really starting to look like a proper dropship. I can get started on fabricating parts to assemble the final 2 cradles from scratch. Producing the parts in duplicate should save us a little time and money.</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;b&gt;&lt;color=#F79232&gt;Позволяет высаживать 1 дополнительный мех или танк.&lt;/color&gt;&lt;/b&gt; 
-  Пол дела сделано, босс. Это действительно начинает походить на настоящий дропшип. Я могу приступить к изготовлению с нуля деталей для сборки последних двух подвесных опор. Хорошо, что детали абсолютно одинаковы, это сэкономит нам немного времени и денег.</t>
+Пол дела сделано, босс. Это действительно начинает походить на настоящий дропшип. Я могу приступить к изготовлению с нуля деталей для сборки последних двух подвесных опор. Хорошо, что детали абсолютно одинаковы, это сэкономит нам немного времени и денег.</t>
   </si>
   <si>
     <t>argoUpgrade_DropSlot2.Description.Name</t>
@@ -133,14 +133,14 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;b&gt;&lt;color=#F79232&gt;Enables to Drop 1 additional Mech or Tank.&lt;/color&gt;&lt;/b&gt; 
-  There's more to dropping a lance of BattleMechs from orbit than strapping them to a wall, Commander. Several of the gyros and handling sensors around the ship are damaged or downright missing. If we try to insert the ship from orbit with anything less than an absolutely perfectly balanced load, there's a very real chance we could lose the shuttle and all aboard. We'll need to replace and recalibrate those systems through some test drops before we can make full use of the new Leopard, Commander.
+There's more to dropping a lance of BattleMechs from orbit than strapping them to a wall, Commander. Several of the gyros and handling sensors around the ship are damaged or downright missing. If we try to insert the ship from orbit with anything less than an absolutely perfectly balanced load, there's a very real chance we could lose the shuttle and all aboard. We'll need to replace and recalibrate those systems through some test drops before we can make full use of the new Leopard, Commander.
 ---
 &lt;b&gt;&lt;color=#F79232&gt;Enables to Drop 1 additional Mech or Tank.&lt;/color&gt;&lt;/b&gt; 
  There's more to dropping a lance of BattleMechs from orbit than strapping them to a wall, Commander. Several of the gyros and handling sensors around the ship are damaged or downright missing. If we try to insert the ship from orbit with anything less than an absolutely perfectly balanced load, there's a very real chance we could lose the shuttle and all aboard. We'll need to replace and recalibrate those systems through some test drops before we can make full use of the new Leopard, Commander.</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;b&gt;&lt;color=#F79232&gt;Позволяет высадить 1 дополнительный мех или танк.&lt;/color&gt;&lt;/b&gt; 
-  Чтобы высадить копье мехов с орбиты, недостаточно просто привязать их к стене. Несколько гироскопов и датчиков управления вокруг корабля повреждены или попросту отсутствуют. Если мы попытаемся вывести корабль с орбиты без абсолютно идеально сбалансированной развесовки нагрузки, есть очень даже реальный шанс, что мы потеряем и дропшип и все, что есть у него на борту. Нам нужно будет заменить и откалибровать эти системы при помощи нескольких тестовых высадок, прежде чем мы сможем в полной мере использовать новый «Леопард», командир.</t>
+Чтобы высадить копье мехов с орбиты, недостаточно просто привязать их к стене. Несколько гироскопов и датчиков управления вокруг корабля повреждены или попросту отсутствуют. Если мы попытаемся вывести корабль с орбиты без абсолютно идеально сбалансированной развесовки нагрузки, есть очень даже реальный шанс, что мы потеряем и дропшип и все, что есть у него на борту. Нам нужно будет заменить и откалибровать эти системы при помощи нескольких тестовых высадок, прежде чем мы сможем в полной мере использовать новый «Леопард», командир.</t>
   </si>
   <si>
     <t>argoUpgrade_DropSlot3.Description.Name</t>
@@ -207,7 +207,7 @@
   </si>
   <si>
     <t xml:space="preserve">Множество систем мехотсека &lt;i&gt;«Арго»&lt;/i&gt; предназначались для использования в совокупности со сложной автоматикой времен Звёздной лиги. Перезапуск хотя бы части этой автоматики - это мощная прибавка к нашим техническим возможностям. 
- &lt;b&gt;&lt;color=#F79232&gt;Позволяет второму ремонтному отсеку работать со 100% эффективностью.&lt;/color&gt;&lt;/b&gt;</t>
+&lt;b&gt;&lt;color=#F79232&gt;Позволяет второму ремонтному отсеку работать со 100% эффективностью.&lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t>argoUpgrade_mechBay_automation1.Description.Name</t>
@@ -315,14 +315,14 @@
   </si>
   <si>
     <t xml:space="preserve">The repaired power conduits allow six more 'Mech cubicles to be powered up and made available. This also brings more of the Mech Bay's automated systems online, making Yang's job easier. 
-  &lt;b&gt;&lt;color=#F79232&gt;Enables second Repair bay, allows work on a second 'Mech's at 50% efficiency.&lt;/color&gt;&lt;/b&gt;
+&lt;b&gt;&lt;color=#F79232&gt;Enables second Repair bay, allows work on a second 'Mech's at 50% efficiency.&lt;/color&gt;&lt;/b&gt;
 ---
 The repaired power conduits allow six more 'Mech cubicles to be powered up and made available. This also brings more of the Mech Bay's automated systems online, making Yang's job easier. 
  &lt;b&gt;&lt;color=#F79232&gt;Enables second Repair bay, allows work on a second 'Mech's at 50% efficiency.&lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">Отремонтированная проводка позволяет запустить еще 6 дополнительных платформ для мехов, а также ещё несколько автоматических систем, что серьезно разгрузит Яна.
-  &lt;b&gt;&lt;color=#F79232&gt;Запускает второй ремонтный отсек, позволяет работать со вторым мехом с 50% эффективностью.&lt;/color&gt;&lt;/b&gt;</t>
+&lt;b&gt;&lt;color=#F79232&gt;Запускает второй ремонтный отсек, позволяет работать со вторым мехом с 50% эффективностью.&lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t>argoUpgrade_mechBay2.Description.Name</t>
@@ -338,14 +338,14 @@
   </si>
   <si>
     <t xml:space="preserve">With the &lt;i&gt;Argo&lt;/i&gt;'s power systems fully online, and enough reinforcement to keep the active Bays from damaging the ship's spine, the final 6 'Mech cubicles can be powered up and put to work. 
-  &lt;b&gt;&lt;color=#F79232&gt;Enables third Repair bay, allows work on a third 'Mech at 33% efficiency.&lt;/color&gt;&lt;/b&gt;.
+&lt;b&gt;&lt;color=#F79232&gt;Enables third Repair bay, allows work on a third 'Mech at 33% efficiency.&lt;/color&gt;&lt;/b&gt;.
 ---
 With the &lt;i&gt;Argo&lt;/i&gt;'s power systems fully online, and enough reinforcement to keep the active Bays from damaging the ship's spine, the final 6 'Mech cubicles can be powered up and put to work. 
  &lt;b&gt;&lt;color=#F79232&gt;Enables third Repair bay, allows work on a third 'Mech at 33% efficiency.&lt;/color&gt;&lt;/b&gt;.</t>
   </si>
   <si>
     <t xml:space="preserve">После вывода систем энергонабжения на полную мощность и усиления «хребта» корабля, достаточного для безопасного функционирования активных мехотсеков, стал возможен ввод в эксплуатацию оставшихся 6 платформ для мехов.
-  &lt;b&gt;&lt;color=#F79232&gt;Запускает третий ремонтный отсек, позволяя работать с третьим мехом с эффективностью 33%&lt;/color&gt;&lt;/b&gt;.</t>
+&lt;b&gt;&lt;color=#F79232&gt;Запускает третий ремонтный отсек, позволяя работать с третьим мехом с эффективностью 33%&lt;/color&gt;&lt;/b&gt;.</t>
   </si>
   <si>
     <t>argoUpgrade_mechBay3.Description.Name</t>
@@ -451,14 +451,14 @@
   </si>
   <si>
     <t xml:space="preserve">Beta Pod, once repaired, includes what was clearly once a hydroponics facility near the spine of the &lt;i&gt;Argo&lt;/i&gt;, and a low-g gymnasium just above that. Neither survived exposure to hard vacuum and stellar radiation, but they're tantalizing indications of the luxuries the &lt;i&gt;Argo&lt;/i&gt; once included. 
-  &lt;b&gt;&lt;color=#F79232&gt;+10 Days before Affinitys Decay. &lt;/color&gt;&lt;/b&gt;
+&lt;b&gt;&lt;color=#F79232&gt;+10 Days before Affinitys Decay. &lt;/color&gt;&lt;/b&gt;
 ---
 Beta Pod, once repaired, includes what was clearly once a hydroponics facility near the spine of the &lt;i&gt;Argo&lt;/i&gt;, and a low-g gymnasium just above that. Neither survived exposure to hard vacuum and stellar radiation, but they're tantalizing indications of the luxuries the &lt;i&gt;Argo&lt;/i&gt; once included. 
  &lt;b&gt;&lt;color=#F79232&gt;+10 Days before Affinitys Decay. &lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">В Отсеке «Бета» находится то, что похоже когда-то было гидропонным садом и спортивным залом с низкой гравитацией прямо над ним. Ни то ни другое не пережило воздействия открытого космоса и звездной радиации, но, тем не менее они являются манящими атрибутами роскошной жизни, которая когда-то была на &lt;i&gt;«Арго»&lt;/i&gt;. 
-  &lt;b&gt;&lt;color=#F79232&gt;+10 дней до начала снижения Affinity.&lt;/color&gt;&lt;/b&gt;</t>
+&lt;b&gt;&lt;color=#F79232&gt;+10 дней до начала снижения Affinity.&lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t>argoUpgrade_pod2.Description.Name</t>
@@ -474,14 +474,14 @@
   </si>
   <si>
     <t xml:space="preserve">Gamma Pod is very much a blank slate, as only its internal support structures survived intact. Rebuilding the habitation decks of the pod still leaves plenty of space for other facilities. 
-  &lt;b&gt;&lt;color=#F79232&gt;+10 Days before Affinitys Decay. &lt;/color&gt;&lt;/b&gt;
+&lt;b&gt;&lt;color=#F79232&gt;+10 Days before Affinitys Decay. &lt;/color&gt;&lt;/b&gt;
 ---
 Gamma Pod is very much a blank slate, as only its internal support structures survived intact. Rebuilding the habitation decks of the pod still leaves plenty of space for other facilities. 
  &lt;b&gt;&lt;color=#F79232&gt;+10 Days before Affinitys Decay. &lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">Отсек «Гамма» - по большому счету - чистый лист, так как нетронутыми остались только его внутренние несущие конструкции. Восстановление жилых палуб отсека оставит в нем много свободного пространства для других объектов.
-  &lt;b&gt;&lt;color=#F79232&gt;+10 дней до начала снижения Affinity.&lt;/color&gt;&lt;/b&gt;</t>
+&lt;b&gt;&lt;color=#F79232&gt;+10 дней до начала снижения Affinity.&lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t>argoUpgrade_pod3.Description.Name</t>
@@ -785,14 +785,14 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;b&gt;&lt;color=#F79232&gt;Reduces the monthly upkeep of all stored inventory items by 5%. This includes equipment, weapons, salvaged 'Mechs and stored 'Mechs.&lt;/color&gt;&lt;/b&gt; 
-  The &lt;i&gt;Argo&lt;/i&gt;'s internal storage is just enough for day-to-day survival, but we'll need to develop an inventory system optimised for the &lt;i&gt;Argo&lt;/i&gt; and not just a standard DropShip. This ship's layout and functions are so different from standard that a new unified inventory system needs to be developed from scratch.
+The &lt;i&gt;Argo&lt;/i&gt;'s internal storage is just enough for day-to-day survival, but we'll need to develop an inventory system optimised for the &lt;i&gt;Argo&lt;/i&gt; and not just a standard DropShip. This ship's layout and functions are so different from standard that a new unified inventory system needs to be developed from scratch.
 ---
 &lt;b&gt;&lt;color=#F79232&gt;Reduces the monthly upkeep of all stored inventory items by 5%. This includes equipment, weapons, salvaged 'Mechs and stored 'Mechs.&lt;/color&gt;&lt;/b&gt; 
  The &lt;i&gt;Argo&lt;/i&gt;'s internal storage is just enough for day-to-day survival, but we'll need to develop an inventory system optimised for the  &lt;i&gt;Argo&lt;/i&gt; and not just a standard DropShip. This ship's layout and functions are so different from standard that a new unified inventory system needs to be developed from scratch.</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;b&gt;&lt;color=#F79232&gt;Сокращает ежемесячные расходы на хранение запасов на 5%. Включает в себя оборудование, оружие, разобранные и собранные мехи.&lt;/color&gt;&lt;/b&gt; 
-  Внутреннего хранилища &lt;i&gt;«Арго»&lt;/i&gt; вполне достаточно для повседневной жизни, но нам нужно разработать систему инвентаризации, оптимизированную именно под &lt;i&gt;«Арго»&lt;/i&gt;, а не просто под какой-то стандартный дропшип. Компоновка и функции этого корабля настолько отличаются от стандартных, что новую унифицированную систему инвентаризации нужно разрабатывать с нуля.</t>
+Внутреннего хранилища &lt;i&gt;«Арго»&lt;/i&gt; вполне достаточно для повседневной жизни, но нам нужно разработать систему инвентаризации, оптимизированную именно под &lt;i&gt;«Арго»&lt;/i&gt;, а не просто под какой-то стандартный дропшип. Компоновка и функции этого корабля настолько отличаются от стандартных, что новую унифицированную систему инвентаризации нужно разрабатывать с нуля.</t>
   </si>
   <si>
     <t>argoUpgrade_storage.Description.Name</t>
@@ -808,14 +808,14 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;b&gt;&lt;color=#F79232&gt;Reduces the monthly upkeep of all stored inventory items by 5%. This includes equipment, weapons, salvaged 'Mechs and stored 'Mechs.&lt;/color&gt;&lt;/b&gt; 
-  An optimised inventory system for the &lt;i&gt;Argo&lt;/i&gt; is an excellent start, but we can cut storage costs further. If you're willing to front the cost for a few, rugged WorkMechs, we'd save a ton of labour and time managing our storage. This will translate into cheaper storage costs in the long run.
+An optimised inventory system for the &lt;i&gt;Argo&lt;/i&gt; is an excellent start, but we can cut storage costs further. If you're willing to front the cost for a few, rugged WorkMechs, we'd save a ton of labour and time managing our storage. This will translate into cheaper storage costs in the long run.
 ---
 &lt;b&gt;&lt;color=#F79232&gt;Reduces the monthly upkeep of all stored inventory items by 5%. This includes equipment, weapons, salvaged 'Mechs and stored 'Mechs.&lt;/color&gt;&lt;/b&gt; 
  An optimised inventory system for the &lt;i&gt;Argo&lt;/i&gt; is an excellent start, but we can cut storage costs further. If you're willing to front the cost for a few, rugged WorkMechs, we'd save a ton of labour and time managing our storage. This will translate into cheaper storage costs in the long run.</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;b&gt;&lt;color=#F79232&gt;Сокращает ежемесячные расходы на хранение запасов на 5%. Включает в себя оборудование, оружие, разобранные и собранные мехи.&lt;/color&gt;&lt;/b&gt; 
-  Оптимизированная система инвентаризации &lt;i&gt;«Арго»&lt;/i&gt; - прекрасное начало, но мы можем сократить расходы на хранение еще больше. Если вы готовы оплатить стоимость нескольких крепких рабочих мехов, мы сэкономим массу времени и сил на управление хранилищами. Это приведет к снижению затрат на хранение в долгосрочной перспективе.</t>
+Оптимизированная система инвентаризации &lt;i&gt;«Арго»&lt;/i&gt; - прекрасное начало, но мы можем сократить расходы на хранение еще больше. Если вы готовы оплатить стоимость нескольких крепких рабочих мехов, мы сэкономим массу времени и сил на управление хранилищами. Это приведет к снижению затрат на хранение в долгосрочной перспективе.</t>
   </si>
   <si>
     <t>argoUpgrade_storage2.Description.Name</t>
@@ -825,14 +825,14 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;b&gt;&lt;color=#F79232&gt;Reduces the monthly upkeep of all stored inventory items by 5%. This includes equipment, weapons, salvaged 'Mechs and stored 'Mechs.&lt;/color&gt;&lt;/b&gt; 
-  Automating the &lt;i&gt;Argo&lt;/i&gt;'s internal storage is the future. One last upgrade to the storage cells would let us move to an automated drone inventory system with a few pressurised WorkMechs for special work. Depressurising some of our inventory and making robots do the work will save us a lot of upkeep by letting us assign the labour and resources elsewhere
+Automating the &lt;i&gt;Argo&lt;/i&gt;'s internal storage is the future. One last upgrade to the storage cells would let us move to an automated drone inventory system with a few pressurised WorkMechs for special work. Depressurising some of our inventory and making robots do the work will save us a lot of upkeep by letting us assign the labour and resources elsewhere
 ---
 &lt;b&gt;&lt;color=#F79232&gt;Reduces the monthly upkeep of all stored inventory items by 5%. This includes equipment, weapons, salvaged 'Mechs and stored 'Mechs.&lt;/color&gt;&lt;/b&gt; 
  Automating the &lt;i&gt;Argo&lt;/i&gt;'s internal storage is the future. One last upgrade to the storage cells would let us move to an automated drone inventory system with a few pressurised WorkMechs for special work. Depressurising some of our inventory and making robots do the work will save us a lot of upkeep by letting us assign the labour and resources elsewhere</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;b&gt;&lt;color=#F79232&gt;Сокращает ежемесячные расходы на хранение запасов на 5%. Включает в себя оборудование, оружие, разобранные и собранные мехи.&lt;/color&gt;&lt;/b&gt; 
-  За автоматизацией внутреннего хранилища &lt;i&gt;«Арго»&lt;/i&gt; будущее. Последнее улучшение ячеек хранения позволит нам перейти на инвентаризационную систему, использующую автоматические дроны в купе с парой герметичных рабочих мехов для доп. работ. Разгерметизация некоторых отсеков хранилища и использование там роботов позволит сэкономить много ресурсов, которые мы сможем перераспределить куда-то ещё.</t>
+За автоматизацией внутреннего хранилища &lt;i&gt;«Арго»&lt;/i&gt; будущее. Последнее улучшение ячеек хранения позволит нам перейти на инвентаризационную систему, использующую автоматические дроны в купе с парой герметичных рабочих мехов для доп. работ. Разгерметизация некоторых отсеков хранилища и использование там роботов позволит сэкономить много ресурсов, которые мы сможем перераспределить куда-то ещё.</t>
   </si>
   <si>
     <t>argoUpgrade_storage3.Description.Name</t>
@@ -842,8 +842,8 @@
   </si>
   <si>
     <t xml:space="preserve">This set of networked Battle Pods allow MechWarriors to compete against one another in simulated 'Mech battles, generating experience for participating MechWarriors. 
-  &lt;b&gt;&lt;color=#F79232&gt;Each MechWarrior with less than 200,000 total experience will gain 30 experience points per day. &lt;/color&gt;&lt;/b&gt; 
-  &lt;b&gt;&lt;color=#F79232&gt;Affinity decays to minimum 5 points&lt;/color&gt;&lt;/b&gt;
+&lt;b&gt;&lt;color=#F79232&gt;Each MechWarrior with less than 200,000 total experience will gain 30 experience points per day. &lt;/color&gt;&lt;/b&gt; 
+&lt;b&gt;&lt;color=#F79232&gt;Affinity decays to minimum 5 points&lt;/color&gt;&lt;/b&gt;
 ---
 This set of networked Battle Pods allow MechWarriors to compete against one another in simulated 'Mech battles, generating experience for participating MechWarriors.  
  &lt;b&gt;&lt;color=#F79232&gt;Each MechWarrior with less than 200,000 total experience will gain 30 experience points per day. &lt;/color&gt;&lt;/b&gt; 
@@ -851,8 +851,8 @@
   </si>
   <si>
     <t xml:space="preserve">Этот набор соединённых локальной сетью боевых модулей позволит мехвоинам получить дополнительный опыт, проводя симуляции сражений друг с другом на мехах.
-  &lt;b&gt;&lt;color=#F79232&gt;Каждый мехвоин с общим количеством опыта менее 200 000 будет получать по 30 очков опыта в день. &lt;/color&gt;&lt;/b&gt; 
-  &lt;b&gt;&lt;color=#F79232&gt;Affinity не опустится ниже 5 единиц.&lt;/color&gt;&lt;/b&gt;</t>
+&lt;b&gt;&lt;color=#F79232&gt;Каждый мехвоин с общим количеством опыта менее 200 000 будет получать по 30 очков опыта в день. &lt;/color&gt;&lt;/b&gt; 
+&lt;b&gt;&lt;color=#F79232&gt;Affinity не опустится ниже 5 единиц.&lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t>argoUpgrade_trainingModule1.Description.Name</t>
@@ -868,8 +868,8 @@
   </si>
   <si>
     <t xml:space="preserve">Adding more Battle Pods allows for full-lance training simulations, as well as raucous ship-wide tournaments. This increases the amount of experience gained by MechWarriors aboard the ship. 
-  &lt;b&gt;&lt;color=#F79232&gt;Each MechWarrior with less than 500,000 total experience will gain 50 experience points per day. &lt;/color&gt;&lt;/b&gt; 
-  &lt;b&gt;&lt;color=#F79232&gt;Affinity decays to minimum 10 points &lt;/color&gt;&lt;/b&gt;
+&lt;b&gt;&lt;color=#F79232&gt;Each MechWarrior with less than 500,000 total experience will gain 50 experience points per day. &lt;/color&gt;&lt;/b&gt; 
+&lt;b&gt;&lt;color=#F79232&gt;Affinity decays to minimum 10 points &lt;/color&gt;&lt;/b&gt;
 ---
 Adding more Battle Pods allows for full-lance training simulations, as well as raucous ship-wide tournaments. This increases the amount of experience gained by MechWarriors aboard the ship.  
  &lt;b&gt;&lt;color=#F79232&gt;Each MechWarrior with less than 500,000 total experience will gain 50 experience points per day. &lt;/color&gt;&lt;/b&gt; 
@@ -877,8 +877,8 @@
   </si>
   <si>
     <t xml:space="preserve">Увеличение количества боевых капсул позволит проводить как полноценные тренировочные симуляции целым копьём, так и всеми любимые внутрикорабельные турниры. Это сильно повысит опыт, приобретаемый мехвоинами на борту корабля.
-  &lt;b&gt;&lt;color=#F79232&gt;Каждый мехвоин с общим количеством опыта менее 500 000 будет получать по 50 очков опыта в день.&lt;/color&gt;&lt;/b&gt; 
-  &lt;b&gt;&lt;color=#F79232&gt;Affinity не опустится ниже 10 единиц.&lt;/color&gt;&lt;/b&gt;</t>
+&lt;b&gt;&lt;color=#F79232&gt;Каждый мехвоин с общим количеством опыта менее 500 000 будет получать по 50 очков опыта в день.&lt;/color&gt;&lt;/b&gt; 
+&lt;b&gt;&lt;color=#F79232&gt;Affinity не опустится ниже 10 единиц.&lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t>argoUpgrade_trainingModule2.Description.Name</t>
@@ -894,8 +894,8 @@
   </si>
   <si>
     <t xml:space="preserve">With a training space completely packed with Battle Pods, MechWarriors can engage in lance-versus-lance competition, and that inevitably means teams, logos, and pennants. Large-scale competition means even more experience for participating MechWarriors. 
-  &lt;b&gt;&lt;color=#F79232&gt;Each MechWarrior with less than 800,000 total experience will gain 80 experience points per day.&lt;/color&gt;&lt;/b&gt; 
-  &lt;b&gt;&lt;color=#F79232&gt;Affinity decays to minimum 40 points &lt;/color&gt;&lt;/b&gt;
+&lt;b&gt;&lt;color=#F79232&gt;Each MechWarrior with less than 800,000 total experience will gain 80 experience points per day.&lt;/color&gt;&lt;/b&gt; 
+&lt;b&gt;&lt;color=#F79232&gt;Affinity decays to minimum 40 points &lt;/color&gt;&lt;/b&gt;
 ---
 With a training space completely packed with Battle Pods, MechWarriors can engage in lance-versus-lance competition, and that inevitably means teams, logos, and pennants. Large-scale competition means even more experience for participating MechWarriors.  
  &lt;b&gt;&lt;color=#F79232&gt;Each MechWarrior with less than 800,000 total experience will gain 80 experience points per day.&lt;/color&gt;&lt;/b&gt; 
@@ -903,8 +903,8 @@
   </si>
   <si>
     <t xml:space="preserve">С тренировочным комплексом, полностью укомплектованным боевыми модулями, мехвоины смогут сражаться «копье на копье», что неминуемо приведет к возникновению команд, логотипов и вымпелов. Широкомасшабная конкуренция даст еще больше опыта участвующим мехвоинам.
-  &lt;b&gt;&lt;color=#F79232&gt;Каждый мехвоин с общим количеством опыта менее 800,000 будет получать по 80 очков опыта в день.&lt;/color&gt;&lt;/b&gt; 
-  &lt;b&gt;&lt;color=#F79232&gt;Affinity не опустится ниже 40 единиц.&lt;/color&gt;&lt;/b&gt;</t>
+&lt;b&gt;&lt;color=#F79232&gt;Каждый мехвоин с общим количеством опыта менее 800,000 будет получать по 80 очков опыта в день.&lt;/color&gt;&lt;/b&gt; 
+&lt;b&gt;&lt;color=#F79232&gt;Affinity не опустится ниже 40 единиц.&lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t>argoUpgrade_trainingModule3.Description.Name</t>
@@ -920,14 +920,14 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;b&gt;&lt;color=#F79232&gt;Allows you to Drop an Additional Vehicle&lt;/color&gt;&lt;/b&gt; 
-  The Command and Control systems were never really intended to support a Light Company’s worth of ‘Mechs, Commander. If we want to maintain communications with our pilots, we’ll need to upgrade our communication networks to deal with the additional bandwidth.
+The Command and Control systems were never really intended to support a Light Company’s worth of ‘Mechs, Commander. If we want to maintain communications with our pilots, we’ll need to upgrade our communication networks to deal with the additional bandwidth.
 ---
 &lt;b&gt;&lt;color=#F79232&gt;Allows you to Drop an Additional Vehicle&lt;/color&gt;&lt;/b&gt; 
  The Command and Control systems were never really intended to support a Light Company’s worth of ‘Mechs, Commander. If we want to maintain communications with our pilots, we’ll need to upgrade our communication networks to deal with the additional bandwidth.</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;b&gt;&lt;color=#F79232&gt;Позволяет высаживать дополнительную единицу техники.&lt;/color&gt;&lt;/b&gt; 
-  Командир, системы управления и контроля никогда не предназначались для поддержки малобюджетных кампаний, у которых на вооружении лишь танки и лёгкие мехи. Если мы хотим поддерживать связь с нашими пилотами, нам нужно улучшить пропускную способность наших коммуникационных сетей.</t>
+Командир, системы управления и контроля никогда не предназначались для поддержки малобюджетных кампаний, у которых на вооружении лишь танки и лёгкие мехи. Если мы хотим поддерживать связь с нашими пилотами, нам нужно улучшить пропускную способность наших коммуникационных сетей.</t>
   </si>
   <si>
     <t>argoUpgrade_VehicleSlot.Description.Name</t>
@@ -943,14 +943,14 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;b&gt;&lt;color=#F79232&gt;Allows you to Drop an Additional Vehicle&lt;/color&gt;&lt;/b&gt; 
-  The upgrades continue commander. Interfacing this Star League technology with our own C&amp;C systems is proving challenging, but there's no problem more money and time can't fix, right?
+The upgrades continue commander. Interfacing this Star League technology with our own C&amp;C systems is proving challenging, but there's no problem more money and time can't fix, right?
 ---
 &lt;b&gt;&lt;color=#F79232&gt;Allows you to Drop an Additional Vehicle&lt;/color&gt;&lt;/b&gt; 
  The upgrades continue commander. Interfacing this Star League technology with our own C&amp;C systems is proving challenging, but there's no problem more money and time can't fix, right?</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;b&gt;&lt;color=#F79232&gt;Позволяет высаживать дополнительную единицу техники.&lt;/color&gt;&lt;/b&gt; 
-  Модернизация продолжается, командир. Наладить взаимодействие между технологией Звёздной лиги и нашей системой управления и контроля будет сложной задачей, но нет таких проблем, которые бы не смогли решить время и деньги, верно?</t>
+Модернизация продолжается, командир. Наладить взаимодействие между технологией Звёздной лиги и нашей системой управления и контроля будет сложной задачей, но нет таких проблем, которые бы не смогли решить время и деньги, верно?</t>
   </si>
   <si>
     <t>argoUpgrade_VehicleSlot1.Description.Name</t>
@@ -969,7 +969,7 @@
   </si>
   <si>
     <t xml:space="preserve">Шаттл бросили ржаветь на свалке, командир. Большинство деталей каркаса &lt;i&gt;«Леопарда»&lt;/i&gt; держатся на ржавчине и честном слове. Мои техи могут приступить к починке самых проблемных участков, но должен предупредить, что на полный ремонт уйдёт очень много времени. 
- &lt;b&gt;&lt;color=#F79232&gt;Увеличивает лимит тоннажа высадки на 50 тонн.&lt;/color&gt;&lt;/b&gt;</t>
+&lt;b&gt;&lt;color=#F79232&gt;Увеличивает лимит тоннажа высадки на 50 тонн.&lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t>argoUpgrade_WeightLimit.Description.Name</t>
@@ -1048,7 +1048,7 @@
   </si>
   <si>
     <t xml:space="preserve">Теперь, когда двигатели и структура корабля восстановлены, следующим шагом будет откалибровать системы управления, чтобы они учитывали изменения в балансе и производительности после нашего ремонта . Нам нужно совершить серию орбитальных высадок для точного измерения характеристик управляемости, а затем внести изменения в бортовые системы управления полетом.
- &lt;b&gt;&lt;color=#F79232&gt;Увеличивает лимит тоннажа высадки на 50 тонн.&lt;/color&gt;&lt;/b&gt;</t>
+&lt;b&gt;&lt;color=#F79232&gt;Увеличивает лимит тоннажа высадки на 50 тонн.&lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t>argoUpgrade_WeightLimit6.Description.Name</t>
@@ -1061,7 +1061,7 @@
   </si>
   <si>
     <t xml:space="preserve">Хорошая новость - мы почти на финишной прямой! Честно говоря, я никогда не думал, что мы продвинемся так далеко, босс. Я откладывал этот разговор до этого момента из-за хронического недостатка времени и денег, но хребет корабля погнут. Он погнулся либо во время со своей предыдущей службы, либо когда гнил на свалке. Нам придется полностью разобрать корабль до основания, чтобы починить его, зато потом он будет как новенький! 
- &lt;b&gt;&lt;color=#F79232&gt;Увеличивает лимит тоннажа высадки на 50 тонн.&lt;/color&gt;&lt;/b&gt;</t>
+&lt;b&gt;&lt;color=#F79232&gt;Увеличивает лимит тоннажа высадки на 50 тонн.&lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t>argoUpgrade_WeightLimit7.Description.Name</t>
@@ -1103,11 +1103,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="2" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="2" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="2" applyFill="1" borderId="0" applyBorder="1" xfId="0" quotePrefix="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1403,18 +1409,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H114"/>
+  <dimension ref="A1:G114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C114"/>
+    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="27.7109375" customWidth="1" style="2"/>
     <col min="2" max="3" width="94.5703125" customWidth="1" style="2"/>
-    <col min="4" max="7" width="9.140625" customWidth="1" style="2"/>
-    <col min="8" max="16384" width="9.140625" customWidth="1" style="2"/>
+    <col min="4" max="6" width="9.140625" customWidth="1" style="2"/>
+    <col min="7" max="16384" width="9.140625" customWidth="1" style="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1472,35 +1478,33 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" s="3" customFormat="1">
-      <c r="A6" s="3" t="s">
+    <row r="6" s="4" customFormat="1">
+      <c r="A6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="H6" s="3"/>
-    </row>
-    <row r="7" s="3" customFormat="1">
-      <c r="A7" s="3" t="s">
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" ht="90" s="4" customFormat="1">
+      <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="H7" s="3"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="G7" s="4"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
@@ -1513,20 +1517,19 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" s="3" customFormat="1">
-      <c r="A9" s="3" t="s">
+    <row r="9" ht="75" s="4" customFormat="1">
+      <c r="A9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="H9" s="3"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="G9" s="4"/>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
@@ -1539,20 +1542,19 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" s="3" customFormat="1">
-      <c r="A11" s="3" t="s">
+    <row r="11" ht="75" s="4" customFormat="1">
+      <c r="A11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="H11" s="3"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="G11" s="4"/>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
@@ -1565,20 +1567,19 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" s="3" customFormat="1">
-      <c r="A13" s="3" t="s">
+    <row r="13" ht="120" s="4" customFormat="1">
+      <c r="A13" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="H13" s="3"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="G13" s="4"/>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
@@ -1657,14 +1658,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" ht="75">
       <c r="A21" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="3" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1723,20 +1724,19 @@
         <v>71</v>
       </c>
     </row>
-    <row r="27" s="3" customFormat="1">
-      <c r="A27" s="3" t="s">
+    <row r="27" s="4" customFormat="1">
+      <c r="A27" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="H27" s="3"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="G27" s="4"/>
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
@@ -1793,20 +1793,19 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" s="3" customFormat="1">
-      <c r="A33" s="3" t="s">
+    <row r="33" ht="75" s="4" customFormat="1">
+      <c r="A33" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="H33" s="3"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="G33" s="4"/>
     </row>
     <row r="34">
       <c r="A34" s="2" t="s">
@@ -1819,20 +1818,19 @@
         <v>95</v>
       </c>
     </row>
-    <row r="35" s="3" customFormat="1">
-      <c r="A35" s="3" t="s">
+    <row r="35" ht="90" s="4" customFormat="1">
+      <c r="A35" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="H35" s="3"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="G35" s="4"/>
     </row>
     <row r="36">
       <c r="A36" s="2" t="s">
@@ -1955,20 +1953,19 @@
         <v>131</v>
       </c>
     </row>
-    <row r="47" s="3" customFormat="1">
-      <c r="A47" s="3" t="s">
+    <row r="47" ht="90" s="4" customFormat="1">
+      <c r="A47" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C47" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="H47" s="3"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="G47" s="4"/>
     </row>
     <row r="48">
       <c r="A48" s="2" t="s">
@@ -1981,20 +1978,19 @@
         <v>137</v>
       </c>
     </row>
-    <row r="49" s="3" customFormat="1">
-      <c r="A49" s="3" t="s">
+    <row r="49" ht="60" s="4" customFormat="1">
+      <c r="A49" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C49" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="H49" s="3"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="G49" s="4"/>
     </row>
     <row r="50">
       <c r="A50" s="2" t="s">
@@ -2359,20 +2355,19 @@
         <v>239</v>
       </c>
     </row>
-    <row r="83" s="3" customFormat="1">
-      <c r="A83" s="3" t="s">
+    <row r="83" ht="120" s="4" customFormat="1">
+      <c r="A83" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="B83" s="3" t="s">
+      <c r="B83" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="C83" s="3" t="s">
+      <c r="C83" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="D83" s="3"/>
-      <c r="E83" s="3"/>
-      <c r="F83" s="3"/>
-      <c r="H83" s="3"/>
+      <c r="D83" s="4"/>
+      <c r="E83" s="4"/>
+      <c r="G83" s="4"/>
     </row>
     <row r="84">
       <c r="A84" s="2" t="s">
@@ -2385,20 +2380,19 @@
         <v>245</v>
       </c>
     </row>
-    <row r="85" s="3" customFormat="1">
-      <c r="A85" s="3" t="s">
+    <row r="85" ht="105" s="4" customFormat="1">
+      <c r="A85" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="B85" s="3" t="s">
+      <c r="B85" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="C85" s="3" t="s">
+      <c r="C85" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="D85" s="3"/>
-      <c r="E85" s="3"/>
-      <c r="F85" s="3"/>
-      <c r="H85" s="3"/>
+      <c r="D85" s="4"/>
+      <c r="E85" s="4"/>
+      <c r="G85" s="4"/>
     </row>
     <row r="86">
       <c r="A86" s="2" t="s">
@@ -2411,20 +2405,19 @@
         <v>245</v>
       </c>
     </row>
-    <row r="87" s="3" customFormat="1">
-      <c r="A87" s="3" t="s">
+    <row r="87" ht="120" s="4" customFormat="1">
+      <c r="A87" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="B87" s="3" t="s">
+      <c r="B87" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="C87" s="3" t="s">
+      <c r="C87" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="D87" s="3"/>
-      <c r="E87" s="3"/>
-      <c r="F87" s="3"/>
-      <c r="H87" s="3"/>
+      <c r="D87" s="4"/>
+      <c r="E87" s="4"/>
+      <c r="G87" s="4"/>
     </row>
     <row r="88">
       <c r="A88" s="2" t="s">
@@ -2437,20 +2430,19 @@
         <v>245</v>
       </c>
     </row>
-    <row r="89" s="3" customFormat="1">
-      <c r="A89" s="3" t="s">
+    <row r="89" ht="105" s="4" customFormat="1">
+      <c r="A89" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="B89" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="C89" s="3" t="s">
+      <c r="C89" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="D89" s="3"/>
-      <c r="E89" s="3"/>
-      <c r="F89" s="3"/>
-      <c r="H89" s="3"/>
+      <c r="D89" s="4"/>
+      <c r="E89" s="4"/>
+      <c r="G89" s="4"/>
     </row>
     <row r="90">
       <c r="A90" s="2" t="s">
@@ -2463,20 +2455,19 @@
         <v>259</v>
       </c>
     </row>
-    <row r="91" s="3" customFormat="1">
-      <c r="A91" s="3" t="s">
+    <row r="91" ht="120" s="4" customFormat="1">
+      <c r="A91" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="B91" s="3" t="s">
+      <c r="B91" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="C91" s="3" t="s">
+      <c r="C91" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="D91" s="3"/>
-      <c r="E91" s="3"/>
-      <c r="F91" s="3"/>
-      <c r="H91" s="3"/>
+      <c r="D91" s="4"/>
+      <c r="E91" s="4"/>
+      <c r="G91" s="4"/>
     </row>
     <row r="92">
       <c r="A92" s="2" t="s">
@@ -2489,20 +2480,19 @@
         <v>265</v>
       </c>
     </row>
-    <row r="93" s="3" customFormat="1">
-      <c r="A93" s="3" t="s">
+    <row r="93" ht="120" s="4" customFormat="1">
+      <c r="A93" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="B93" s="3" t="s">
+      <c r="B93" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="C93" s="3" t="s">
+      <c r="C93" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="D93" s="3"/>
-      <c r="E93" s="3"/>
-      <c r="F93" s="3"/>
-      <c r="H93" s="3"/>
+      <c r="D93" s="4"/>
+      <c r="E93" s="4"/>
+      <c r="G93" s="4"/>
     </row>
     <row r="94">
       <c r="A94" s="2" t="s">
@@ -2515,20 +2505,19 @@
         <v>271</v>
       </c>
     </row>
-    <row r="95" s="3" customFormat="1">
-      <c r="A95" s="3" t="s">
+    <row r="95" ht="90" s="4" customFormat="1">
+      <c r="A95" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="B95" s="3" t="s">
+      <c r="B95" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="C95" s="3" t="s">
+      <c r="C95" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="D95" s="3"/>
-      <c r="E95" s="3"/>
-      <c r="F95" s="3"/>
-      <c r="H95" s="3"/>
+      <c r="D95" s="4"/>
+      <c r="E95" s="4"/>
+      <c r="G95" s="4"/>
     </row>
     <row r="96">
       <c r="A96" s="2" t="s">
@@ -2541,20 +2530,19 @@
         <v>277</v>
       </c>
     </row>
-    <row r="97" s="3" customFormat="1">
-      <c r="A97" s="3" t="s">
+    <row r="97" ht="75" s="4" customFormat="1">
+      <c r="A97" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="B97" s="3" t="s">
+      <c r="B97" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="C97" s="3" t="s">
+      <c r="C97" s="5" t="s">
         <v>280</v>
       </c>
-      <c r="D97" s="3"/>
-      <c r="E97" s="3"/>
-      <c r="F97" s="3"/>
-      <c r="H97" s="3"/>
+      <c r="D97" s="4"/>
+      <c r="E97" s="4"/>
+      <c r="G97" s="4"/>
     </row>
     <row r="98">
       <c r="A98" s="2" t="s">
@@ -2567,14 +2555,14 @@
         <v>283</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" ht="60">
       <c r="A99" s="2" t="s">
         <v>284</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="C99" s="2" t="s">
+      <c r="C99" s="3" t="s">
         <v>286</v>
       </c>
     </row>
@@ -2699,14 +2687,14 @@
         <v>289</v>
       </c>
     </row>
-    <row r="111">
+    <row r="111" ht="90">
       <c r="A111" s="2" t="s">
         <v>310</v>
       </c>
       <c r="B111" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="C111" s="2" t="s">
+      <c r="C111" s="3" t="s">
         <v>312</v>
       </c>
     </row>
@@ -2721,14 +2709,14 @@
         <v>289</v>
       </c>
     </row>
-    <row r="113">
+    <row r="113" ht="90">
       <c r="A113" s="2" t="s">
         <v>314</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="C113" s="2" t="s">
+      <c r="C113" s="3" t="s">
         <v>316</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "Revert "New Russian Localisation""
This reverts commit 6b963ab7fb5181a7401a54b6189b3bf88c602a5f.
</commit_message>
<xml_diff>
--- a/CustomLocalization/Localization/RogueTech/RU/Argo Upg/LocalizationDef.xlsx
+++ b/CustomLocalization/Localization/RogueTech/RU/Argo Upg/LocalizationDef.xlsx
@@ -76,14 +76,14 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;b&gt;&lt;color=#F79232&gt;Enables to Drop 1 additional Mech or Tank.&lt;/color&gt;&lt;/b&gt; 
-So it turns out the docking cradles were salvaged for parts and scrap, but the mounting points are still intact. I can get my techs to work fabricating new 'Mech cradles commander, but it's gonna take a while to get everything rebuilt. I think there's enough pieces left behind to get one assembled quickly, though.
+  So it turns out the docking cradles were salvaged for parts and scrap, but the mounting points are still intact. I can get my techs to work fabricating new 'Mech cradles commander, but it's gonna take a while to get everything rebuilt. I think there's enough pieces left behind to get one assembled quickly, though.
 ---
 &lt;b&gt;&lt;color=#F79232&gt;Enables to Drop 1 additional Mech or Tank.&lt;/color&gt;&lt;/b&gt; 
  So it turns out the docking cradles were salvaged for parts and scrap, but the mounting points are still intact. I can get my techs to work fabricating new 'Mech cradles commander, but it's gonna take a while to get everything rebuilt. I think there's enough pieces left behind to get one assembled quickly, though.</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;b&gt;&lt;color=#F79232&gt;Позволяет высадить 1 дополнительный мех или танк.&lt;/color&gt;&lt;/b&gt; 
-Похоже, что док-станции были разобраны на запчасти, но места крепления остались невредимы. Я могу попросить моих техов поработать над изготовлением новых док-станций для мехов, командир, но потребуется время, чтобы всё воссоздать заново. Хотя, думаю, тут валяется достаточно частей, чтобы быстро собрать хотя бы одну из них.</t>
+  Похоже, что док-станции были разобраны на запчасти, но места крепления остались невредимы. Я могу попросить моих техов поработать над изготовлением новых док-станций для мехов, командир, но потребуется время, чтобы всё воссоздать заново. Хотя, думаю, тут валяется достаточно частей, чтобы быстро собрать хотя бы одну из них.</t>
   </si>
   <si>
     <t>argoUpgrade_DropSlot.Description.Name</t>
@@ -99,14 +99,14 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;b&gt;&lt;color=#F79232&gt;Enables to Drop 1 additional Mech or Tank.&lt;/color&gt;&lt;/b&gt; 
-The first cradle turned out alright, Boss. There's enough scrap left lying around we should be able to construct the bones of a gantry for the next, but we're also gonna need to buy several complex components to get the next cradle ready for use.
+  The first cradle turned out alright, Boss. There's enough scrap left lying around we should be able to construct the bones of a gantry for the next, but we're also gonna need to buy several complex components to get the next cradle ready for use.
 ---
 &lt;b&gt;&lt;color=#F79232&gt;Enables to Drop 1 additional Mech or Tank.&lt;/color&gt;&lt;/b&gt; 
  The first cradle turned out alright, Boss. There's enough scrap left lying around we should be able to construct the bones of a gantry for the next, but we're also gonna need to buy several complex components to get the next cradle ready for use.</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;b&gt;&lt;color=#F79232&gt;Позволяет высадить 1 дополнительный мех или танк.&lt;/color&gt;&lt;/b&gt; 
-Первая док-станция в порядке, босс. Вокруг осталось достаточно металлолома, чтобы мы могли соорудить каркас для ещё одной, но нам точно нужно закупить ещё несколько сложных компонентов, чтобы подготовить док-станцию к использованию.</t>
+  Первая док-станция в порядке, босс. Вокруг осталось достаточно металлолома, чтобы мы могли соорудить каркас для ещё одной, но нам точно нужно закупить ещё несколько сложных компонентов, чтобы подготовить док-станцию к использованию.</t>
   </si>
   <si>
     <t>argoUpgrade_DropSlot1.Description.Name</t>
@@ -116,14 +116,14 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;b&gt;&lt;color=#F79232&gt;Enables to Drop 1 additional Mech or Tank.&lt;/color&gt;&lt;/b&gt; 
-Half-done now, Boss. It's really starting to look like a proper dropship. I can get started on fabricating parts to assemble the final 2 cradles from scratch. Producing the parts in duplicate should save us a little time and money.
+  Half-done now, Boss. It's really starting to look like a proper dropship. I can get started on fabricating parts to assemble the final 2 cradles from scratch. Producing the parts in duplicate should save us a little time and money.
 ---
 &lt;b&gt;&lt;color=#F79232&gt;Enables to Drop 1 additional Mech or Tank.&lt;/color&gt;&lt;/b&gt; 
  Half-done now, Boss. It's really starting to look like a proper dropship. I can get started on fabricating parts to assemble the final 2 cradles from scratch. Producing the parts in duplicate should save us a little time and money.</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;b&gt;&lt;color=#F79232&gt;Позволяет высаживать 1 дополнительный мех или танк.&lt;/color&gt;&lt;/b&gt; 
-Пол дела сделано, босс. Это действительно начинает походить на настоящий дропшип. Я могу приступить к изготовлению с нуля деталей для сборки последних двух подвесных опор. Хорошо, что детали абсолютно одинаковы, это сэкономит нам немного времени и денег.</t>
+  Пол дела сделано, босс. Это действительно начинает походить на настоящий дропшип. Я могу приступить к изготовлению с нуля деталей для сборки последних двух подвесных опор. Хорошо, что детали абсолютно одинаковы, это сэкономит нам немного времени и денег.</t>
   </si>
   <si>
     <t>argoUpgrade_DropSlot2.Description.Name</t>
@@ -133,14 +133,14 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;b&gt;&lt;color=#F79232&gt;Enables to Drop 1 additional Mech or Tank.&lt;/color&gt;&lt;/b&gt; 
-There's more to dropping a lance of BattleMechs from orbit than strapping them to a wall, Commander. Several of the gyros and handling sensors around the ship are damaged or downright missing. If we try to insert the ship from orbit with anything less than an absolutely perfectly balanced load, there's a very real chance we could lose the shuttle and all aboard. We'll need to replace and recalibrate those systems through some test drops before we can make full use of the new Leopard, Commander.
+  There's more to dropping a lance of BattleMechs from orbit than strapping them to a wall, Commander. Several of the gyros and handling sensors around the ship are damaged or downright missing. If we try to insert the ship from orbit with anything less than an absolutely perfectly balanced load, there's a very real chance we could lose the shuttle and all aboard. We'll need to replace and recalibrate those systems through some test drops before we can make full use of the new Leopard, Commander.
 ---
 &lt;b&gt;&lt;color=#F79232&gt;Enables to Drop 1 additional Mech or Tank.&lt;/color&gt;&lt;/b&gt; 
  There's more to dropping a lance of BattleMechs from orbit than strapping them to a wall, Commander. Several of the gyros and handling sensors around the ship are damaged or downright missing. If we try to insert the ship from orbit with anything less than an absolutely perfectly balanced load, there's a very real chance we could lose the shuttle and all aboard. We'll need to replace and recalibrate those systems through some test drops before we can make full use of the new Leopard, Commander.</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;b&gt;&lt;color=#F79232&gt;Позволяет высадить 1 дополнительный мех или танк.&lt;/color&gt;&lt;/b&gt; 
-Чтобы высадить копье мехов с орбиты, недостаточно просто привязать их к стене. Несколько гироскопов и датчиков управления вокруг корабля повреждены или попросту отсутствуют. Если мы попытаемся вывести корабль с орбиты без абсолютно идеально сбалансированной развесовки нагрузки, есть очень даже реальный шанс, что мы потеряем и дропшип и все, что есть у него на борту. Нам нужно будет заменить и откалибровать эти системы при помощи нескольких тестовых высадок, прежде чем мы сможем в полной мере использовать новый «Леопард», командир.</t>
+  Чтобы высадить копье мехов с орбиты, недостаточно просто привязать их к стене. Несколько гироскопов и датчиков управления вокруг корабля повреждены или попросту отсутствуют. Если мы попытаемся вывести корабль с орбиты без абсолютно идеально сбалансированной развесовки нагрузки, есть очень даже реальный шанс, что мы потеряем и дропшип и все, что есть у него на борту. Нам нужно будет заменить и откалибровать эти системы при помощи нескольких тестовых высадок, прежде чем мы сможем в полной мере использовать новый «Леопард», командир.</t>
   </si>
   <si>
     <t>argoUpgrade_DropSlot3.Description.Name</t>
@@ -207,7 +207,7 @@
   </si>
   <si>
     <t xml:space="preserve">Множество систем мехотсека &lt;i&gt;«Арго»&lt;/i&gt; предназначались для использования в совокупности со сложной автоматикой времен Звёздной лиги. Перезапуск хотя бы части этой автоматики - это мощная прибавка к нашим техническим возможностям. 
-&lt;b&gt;&lt;color=#F79232&gt;Позволяет второму ремонтному отсеку работать со 100% эффективностью.&lt;/color&gt;&lt;/b&gt;</t>
+ &lt;b&gt;&lt;color=#F79232&gt;Позволяет второму ремонтному отсеку работать со 100% эффективностью.&lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t>argoUpgrade_mechBay_automation1.Description.Name</t>
@@ -315,14 +315,14 @@
   </si>
   <si>
     <t xml:space="preserve">The repaired power conduits allow six more 'Mech cubicles to be powered up and made available. This also brings more of the Mech Bay's automated systems online, making Yang's job easier. 
-&lt;b&gt;&lt;color=#F79232&gt;Enables second Repair bay, allows work on a second 'Mech's at 50% efficiency.&lt;/color&gt;&lt;/b&gt;
+  &lt;b&gt;&lt;color=#F79232&gt;Enables second Repair bay, allows work on a second 'Mech's at 50% efficiency.&lt;/color&gt;&lt;/b&gt;
 ---
 The repaired power conduits allow six more 'Mech cubicles to be powered up and made available. This also brings more of the Mech Bay's automated systems online, making Yang's job easier. 
  &lt;b&gt;&lt;color=#F79232&gt;Enables second Repair bay, allows work on a second 'Mech's at 50% efficiency.&lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">Отремонтированная проводка позволяет запустить еще 6 дополнительных платформ для мехов, а также ещё несколько автоматических систем, что серьезно разгрузит Яна.
-&lt;b&gt;&lt;color=#F79232&gt;Запускает второй ремонтный отсек, позволяет работать со вторым мехом с 50% эффективностью.&lt;/color&gt;&lt;/b&gt;</t>
+  &lt;b&gt;&lt;color=#F79232&gt;Запускает второй ремонтный отсек, позволяет работать со вторым мехом с 50% эффективностью.&lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t>argoUpgrade_mechBay2.Description.Name</t>
@@ -338,14 +338,14 @@
   </si>
   <si>
     <t xml:space="preserve">With the &lt;i&gt;Argo&lt;/i&gt;'s power systems fully online, and enough reinforcement to keep the active Bays from damaging the ship's spine, the final 6 'Mech cubicles can be powered up and put to work. 
-&lt;b&gt;&lt;color=#F79232&gt;Enables third Repair bay, allows work on a third 'Mech at 33% efficiency.&lt;/color&gt;&lt;/b&gt;.
+  &lt;b&gt;&lt;color=#F79232&gt;Enables third Repair bay, allows work on a third 'Mech at 33% efficiency.&lt;/color&gt;&lt;/b&gt;.
 ---
 With the &lt;i&gt;Argo&lt;/i&gt;'s power systems fully online, and enough reinforcement to keep the active Bays from damaging the ship's spine, the final 6 'Mech cubicles can be powered up and put to work. 
  &lt;b&gt;&lt;color=#F79232&gt;Enables third Repair bay, allows work on a third 'Mech at 33% efficiency.&lt;/color&gt;&lt;/b&gt;.</t>
   </si>
   <si>
     <t xml:space="preserve">После вывода систем энергонабжения на полную мощность и усиления «хребта» корабля, достаточного для безопасного функционирования активных мехотсеков, стал возможен ввод в эксплуатацию оставшихся 6 платформ для мехов.
-&lt;b&gt;&lt;color=#F79232&gt;Запускает третий ремонтный отсек, позволяя работать с третьим мехом с эффективностью 33%&lt;/color&gt;&lt;/b&gt;.</t>
+  &lt;b&gt;&lt;color=#F79232&gt;Запускает третий ремонтный отсек, позволяя работать с третьим мехом с эффективностью 33%&lt;/color&gt;&lt;/b&gt;.</t>
   </si>
   <si>
     <t>argoUpgrade_mechBay3.Description.Name</t>
@@ -451,14 +451,14 @@
   </si>
   <si>
     <t xml:space="preserve">Beta Pod, once repaired, includes what was clearly once a hydroponics facility near the spine of the &lt;i&gt;Argo&lt;/i&gt;, and a low-g gymnasium just above that. Neither survived exposure to hard vacuum and stellar radiation, but they're tantalizing indications of the luxuries the &lt;i&gt;Argo&lt;/i&gt; once included. 
-&lt;b&gt;&lt;color=#F79232&gt;+10 Days before Affinitys Decay. &lt;/color&gt;&lt;/b&gt;
+  &lt;b&gt;&lt;color=#F79232&gt;+10 Days before Affinitys Decay. &lt;/color&gt;&lt;/b&gt;
 ---
 Beta Pod, once repaired, includes what was clearly once a hydroponics facility near the spine of the &lt;i&gt;Argo&lt;/i&gt;, and a low-g gymnasium just above that. Neither survived exposure to hard vacuum and stellar radiation, but they're tantalizing indications of the luxuries the &lt;i&gt;Argo&lt;/i&gt; once included. 
  &lt;b&gt;&lt;color=#F79232&gt;+10 Days before Affinitys Decay. &lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">В Отсеке «Бета» находится то, что похоже когда-то было гидропонным садом и спортивным залом с низкой гравитацией прямо над ним. Ни то ни другое не пережило воздействия открытого космоса и звездной радиации, но, тем не менее они являются манящими атрибутами роскошной жизни, которая когда-то была на &lt;i&gt;«Арго»&lt;/i&gt;. 
-&lt;b&gt;&lt;color=#F79232&gt;+10 дней до начала снижения Affinity.&lt;/color&gt;&lt;/b&gt;</t>
+  &lt;b&gt;&lt;color=#F79232&gt;+10 дней до начала снижения Affinity.&lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t>argoUpgrade_pod2.Description.Name</t>
@@ -474,14 +474,14 @@
   </si>
   <si>
     <t xml:space="preserve">Gamma Pod is very much a blank slate, as only its internal support structures survived intact. Rebuilding the habitation decks of the pod still leaves plenty of space for other facilities. 
-&lt;b&gt;&lt;color=#F79232&gt;+10 Days before Affinitys Decay. &lt;/color&gt;&lt;/b&gt;
+  &lt;b&gt;&lt;color=#F79232&gt;+10 Days before Affinitys Decay. &lt;/color&gt;&lt;/b&gt;
 ---
 Gamma Pod is very much a blank slate, as only its internal support structures survived intact. Rebuilding the habitation decks of the pod still leaves plenty of space for other facilities. 
  &lt;b&gt;&lt;color=#F79232&gt;+10 Days before Affinitys Decay. &lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">Отсек «Гамма» - по большому счету - чистый лист, так как нетронутыми остались только его внутренние несущие конструкции. Восстановление жилых палуб отсека оставит в нем много свободного пространства для других объектов.
-&lt;b&gt;&lt;color=#F79232&gt;+10 дней до начала снижения Affinity.&lt;/color&gt;&lt;/b&gt;</t>
+  &lt;b&gt;&lt;color=#F79232&gt;+10 дней до начала снижения Affinity.&lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t>argoUpgrade_pod3.Description.Name</t>
@@ -785,14 +785,14 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;b&gt;&lt;color=#F79232&gt;Reduces the monthly upkeep of all stored inventory items by 5%. This includes equipment, weapons, salvaged 'Mechs and stored 'Mechs.&lt;/color&gt;&lt;/b&gt; 
-The &lt;i&gt;Argo&lt;/i&gt;'s internal storage is just enough for day-to-day survival, but we'll need to develop an inventory system optimised for the &lt;i&gt;Argo&lt;/i&gt; and not just a standard DropShip. This ship's layout and functions are so different from standard that a new unified inventory system needs to be developed from scratch.
+  The &lt;i&gt;Argo&lt;/i&gt;'s internal storage is just enough for day-to-day survival, but we'll need to develop an inventory system optimised for the &lt;i&gt;Argo&lt;/i&gt; and not just a standard DropShip. This ship's layout and functions are so different from standard that a new unified inventory system needs to be developed from scratch.
 ---
 &lt;b&gt;&lt;color=#F79232&gt;Reduces the monthly upkeep of all stored inventory items by 5%. This includes equipment, weapons, salvaged 'Mechs and stored 'Mechs.&lt;/color&gt;&lt;/b&gt; 
  The &lt;i&gt;Argo&lt;/i&gt;'s internal storage is just enough for day-to-day survival, but we'll need to develop an inventory system optimised for the  &lt;i&gt;Argo&lt;/i&gt; and not just a standard DropShip. This ship's layout and functions are so different from standard that a new unified inventory system needs to be developed from scratch.</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;b&gt;&lt;color=#F79232&gt;Сокращает ежемесячные расходы на хранение запасов на 5%. Включает в себя оборудование, оружие, разобранные и собранные мехи.&lt;/color&gt;&lt;/b&gt; 
-Внутреннего хранилища &lt;i&gt;«Арго»&lt;/i&gt; вполне достаточно для повседневной жизни, но нам нужно разработать систему инвентаризации, оптимизированную именно под &lt;i&gt;«Арго»&lt;/i&gt;, а не просто под какой-то стандартный дропшип. Компоновка и функции этого корабля настолько отличаются от стандартных, что новую унифицированную систему инвентаризации нужно разрабатывать с нуля.</t>
+  Внутреннего хранилища &lt;i&gt;«Арго»&lt;/i&gt; вполне достаточно для повседневной жизни, но нам нужно разработать систему инвентаризации, оптимизированную именно под &lt;i&gt;«Арго»&lt;/i&gt;, а не просто под какой-то стандартный дропшип. Компоновка и функции этого корабля настолько отличаются от стандартных, что новую унифицированную систему инвентаризации нужно разрабатывать с нуля.</t>
   </si>
   <si>
     <t>argoUpgrade_storage.Description.Name</t>
@@ -808,14 +808,14 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;b&gt;&lt;color=#F79232&gt;Reduces the monthly upkeep of all stored inventory items by 5%. This includes equipment, weapons, salvaged 'Mechs and stored 'Mechs.&lt;/color&gt;&lt;/b&gt; 
-An optimised inventory system for the &lt;i&gt;Argo&lt;/i&gt; is an excellent start, but we can cut storage costs further. If you're willing to front the cost for a few, rugged WorkMechs, we'd save a ton of labour and time managing our storage. This will translate into cheaper storage costs in the long run.
+  An optimised inventory system for the &lt;i&gt;Argo&lt;/i&gt; is an excellent start, but we can cut storage costs further. If you're willing to front the cost for a few, rugged WorkMechs, we'd save a ton of labour and time managing our storage. This will translate into cheaper storage costs in the long run.
 ---
 &lt;b&gt;&lt;color=#F79232&gt;Reduces the monthly upkeep of all stored inventory items by 5%. This includes equipment, weapons, salvaged 'Mechs and stored 'Mechs.&lt;/color&gt;&lt;/b&gt; 
  An optimised inventory system for the &lt;i&gt;Argo&lt;/i&gt; is an excellent start, but we can cut storage costs further. If you're willing to front the cost for a few, rugged WorkMechs, we'd save a ton of labour and time managing our storage. This will translate into cheaper storage costs in the long run.</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;b&gt;&lt;color=#F79232&gt;Сокращает ежемесячные расходы на хранение запасов на 5%. Включает в себя оборудование, оружие, разобранные и собранные мехи.&lt;/color&gt;&lt;/b&gt; 
-Оптимизированная система инвентаризации &lt;i&gt;«Арго»&lt;/i&gt; - прекрасное начало, но мы можем сократить расходы на хранение еще больше. Если вы готовы оплатить стоимость нескольких крепких рабочих мехов, мы сэкономим массу времени и сил на управление хранилищами. Это приведет к снижению затрат на хранение в долгосрочной перспективе.</t>
+  Оптимизированная система инвентаризации &lt;i&gt;«Арго»&lt;/i&gt; - прекрасное начало, но мы можем сократить расходы на хранение еще больше. Если вы готовы оплатить стоимость нескольких крепких рабочих мехов, мы сэкономим массу времени и сил на управление хранилищами. Это приведет к снижению затрат на хранение в долгосрочной перспективе.</t>
   </si>
   <si>
     <t>argoUpgrade_storage2.Description.Name</t>
@@ -825,14 +825,14 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;b&gt;&lt;color=#F79232&gt;Reduces the monthly upkeep of all stored inventory items by 5%. This includes equipment, weapons, salvaged 'Mechs and stored 'Mechs.&lt;/color&gt;&lt;/b&gt; 
-Automating the &lt;i&gt;Argo&lt;/i&gt;'s internal storage is the future. One last upgrade to the storage cells would let us move to an automated drone inventory system with a few pressurised WorkMechs for special work. Depressurising some of our inventory and making robots do the work will save us a lot of upkeep by letting us assign the labour and resources elsewhere
+  Automating the &lt;i&gt;Argo&lt;/i&gt;'s internal storage is the future. One last upgrade to the storage cells would let us move to an automated drone inventory system with a few pressurised WorkMechs for special work. Depressurising some of our inventory and making robots do the work will save us a lot of upkeep by letting us assign the labour and resources elsewhere
 ---
 &lt;b&gt;&lt;color=#F79232&gt;Reduces the monthly upkeep of all stored inventory items by 5%. This includes equipment, weapons, salvaged 'Mechs and stored 'Mechs.&lt;/color&gt;&lt;/b&gt; 
  Automating the &lt;i&gt;Argo&lt;/i&gt;'s internal storage is the future. One last upgrade to the storage cells would let us move to an automated drone inventory system with a few pressurised WorkMechs for special work. Depressurising some of our inventory and making robots do the work will save us a lot of upkeep by letting us assign the labour and resources elsewhere</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;b&gt;&lt;color=#F79232&gt;Сокращает ежемесячные расходы на хранение запасов на 5%. Включает в себя оборудование, оружие, разобранные и собранные мехи.&lt;/color&gt;&lt;/b&gt; 
-За автоматизацией внутреннего хранилища &lt;i&gt;«Арго»&lt;/i&gt; будущее. Последнее улучшение ячеек хранения позволит нам перейти на инвентаризационную систему, использующую автоматические дроны в купе с парой герметичных рабочих мехов для доп. работ. Разгерметизация некоторых отсеков хранилища и использование там роботов позволит сэкономить много ресурсов, которые мы сможем перераспределить куда-то ещё.</t>
+  За автоматизацией внутреннего хранилища &lt;i&gt;«Арго»&lt;/i&gt; будущее. Последнее улучшение ячеек хранения позволит нам перейти на инвентаризационную систему, использующую автоматические дроны в купе с парой герметичных рабочих мехов для доп. работ. Разгерметизация некоторых отсеков хранилища и использование там роботов позволит сэкономить много ресурсов, которые мы сможем перераспределить куда-то ещё.</t>
   </si>
   <si>
     <t>argoUpgrade_storage3.Description.Name</t>
@@ -842,8 +842,8 @@
   </si>
   <si>
     <t xml:space="preserve">This set of networked Battle Pods allow MechWarriors to compete against one another in simulated 'Mech battles, generating experience for participating MechWarriors. 
-&lt;b&gt;&lt;color=#F79232&gt;Each MechWarrior with less than 200,000 total experience will gain 30 experience points per day. &lt;/color&gt;&lt;/b&gt; 
-&lt;b&gt;&lt;color=#F79232&gt;Affinity decays to minimum 5 points&lt;/color&gt;&lt;/b&gt;
+  &lt;b&gt;&lt;color=#F79232&gt;Each MechWarrior with less than 200,000 total experience will gain 30 experience points per day. &lt;/color&gt;&lt;/b&gt; 
+  &lt;b&gt;&lt;color=#F79232&gt;Affinity decays to minimum 5 points&lt;/color&gt;&lt;/b&gt;
 ---
 This set of networked Battle Pods allow MechWarriors to compete against one another in simulated 'Mech battles, generating experience for participating MechWarriors.  
  &lt;b&gt;&lt;color=#F79232&gt;Each MechWarrior with less than 200,000 total experience will gain 30 experience points per day. &lt;/color&gt;&lt;/b&gt; 
@@ -851,8 +851,8 @@
   </si>
   <si>
     <t xml:space="preserve">Этот набор соединённых локальной сетью боевых модулей позволит мехвоинам получить дополнительный опыт, проводя симуляции сражений друг с другом на мехах.
-&lt;b&gt;&lt;color=#F79232&gt;Каждый мехвоин с общим количеством опыта менее 200 000 будет получать по 30 очков опыта в день. &lt;/color&gt;&lt;/b&gt; 
-&lt;b&gt;&lt;color=#F79232&gt;Affinity не опустится ниже 5 единиц.&lt;/color&gt;&lt;/b&gt;</t>
+  &lt;b&gt;&lt;color=#F79232&gt;Каждый мехвоин с общим количеством опыта менее 200 000 будет получать по 30 очков опыта в день. &lt;/color&gt;&lt;/b&gt; 
+  &lt;b&gt;&lt;color=#F79232&gt;Affinity не опустится ниже 5 единиц.&lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t>argoUpgrade_trainingModule1.Description.Name</t>
@@ -868,8 +868,8 @@
   </si>
   <si>
     <t xml:space="preserve">Adding more Battle Pods allows for full-lance training simulations, as well as raucous ship-wide tournaments. This increases the amount of experience gained by MechWarriors aboard the ship. 
-&lt;b&gt;&lt;color=#F79232&gt;Each MechWarrior with less than 500,000 total experience will gain 50 experience points per day. &lt;/color&gt;&lt;/b&gt; 
-&lt;b&gt;&lt;color=#F79232&gt;Affinity decays to minimum 10 points &lt;/color&gt;&lt;/b&gt;
+  &lt;b&gt;&lt;color=#F79232&gt;Each MechWarrior with less than 500,000 total experience will gain 50 experience points per day. &lt;/color&gt;&lt;/b&gt; 
+  &lt;b&gt;&lt;color=#F79232&gt;Affinity decays to minimum 10 points &lt;/color&gt;&lt;/b&gt;
 ---
 Adding more Battle Pods allows for full-lance training simulations, as well as raucous ship-wide tournaments. This increases the amount of experience gained by MechWarriors aboard the ship.  
  &lt;b&gt;&lt;color=#F79232&gt;Each MechWarrior with less than 500,000 total experience will gain 50 experience points per day. &lt;/color&gt;&lt;/b&gt; 
@@ -877,8 +877,8 @@
   </si>
   <si>
     <t xml:space="preserve">Увеличение количества боевых капсул позволит проводить как полноценные тренировочные симуляции целым копьём, так и всеми любимые внутрикорабельные турниры. Это сильно повысит опыт, приобретаемый мехвоинами на борту корабля.
-&lt;b&gt;&lt;color=#F79232&gt;Каждый мехвоин с общим количеством опыта менее 500 000 будет получать по 50 очков опыта в день.&lt;/color&gt;&lt;/b&gt; 
-&lt;b&gt;&lt;color=#F79232&gt;Affinity не опустится ниже 10 единиц.&lt;/color&gt;&lt;/b&gt;</t>
+  &lt;b&gt;&lt;color=#F79232&gt;Каждый мехвоин с общим количеством опыта менее 500 000 будет получать по 50 очков опыта в день.&lt;/color&gt;&lt;/b&gt; 
+  &lt;b&gt;&lt;color=#F79232&gt;Affinity не опустится ниже 10 единиц.&lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t>argoUpgrade_trainingModule2.Description.Name</t>
@@ -894,8 +894,8 @@
   </si>
   <si>
     <t xml:space="preserve">With a training space completely packed with Battle Pods, MechWarriors can engage in lance-versus-lance competition, and that inevitably means teams, logos, and pennants. Large-scale competition means even more experience for participating MechWarriors. 
-&lt;b&gt;&lt;color=#F79232&gt;Each MechWarrior with less than 800,000 total experience will gain 80 experience points per day.&lt;/color&gt;&lt;/b&gt; 
-&lt;b&gt;&lt;color=#F79232&gt;Affinity decays to minimum 40 points &lt;/color&gt;&lt;/b&gt;
+  &lt;b&gt;&lt;color=#F79232&gt;Each MechWarrior with less than 800,000 total experience will gain 80 experience points per day.&lt;/color&gt;&lt;/b&gt; 
+  &lt;b&gt;&lt;color=#F79232&gt;Affinity decays to minimum 40 points &lt;/color&gt;&lt;/b&gt;
 ---
 With a training space completely packed with Battle Pods, MechWarriors can engage in lance-versus-lance competition, and that inevitably means teams, logos, and pennants. Large-scale competition means even more experience for participating MechWarriors.  
  &lt;b&gt;&lt;color=#F79232&gt;Each MechWarrior with less than 800,000 total experience will gain 80 experience points per day.&lt;/color&gt;&lt;/b&gt; 
@@ -903,8 +903,8 @@
   </si>
   <si>
     <t xml:space="preserve">С тренировочным комплексом, полностью укомплектованным боевыми модулями, мехвоины смогут сражаться «копье на копье», что неминуемо приведет к возникновению команд, логотипов и вымпелов. Широкомасшабная конкуренция даст еще больше опыта участвующим мехвоинам.
-&lt;b&gt;&lt;color=#F79232&gt;Каждый мехвоин с общим количеством опыта менее 800,000 будет получать по 80 очков опыта в день.&lt;/color&gt;&lt;/b&gt; 
-&lt;b&gt;&lt;color=#F79232&gt;Affinity не опустится ниже 40 единиц.&lt;/color&gt;&lt;/b&gt;</t>
+  &lt;b&gt;&lt;color=#F79232&gt;Каждый мехвоин с общим количеством опыта менее 800,000 будет получать по 80 очков опыта в день.&lt;/color&gt;&lt;/b&gt; 
+  &lt;b&gt;&lt;color=#F79232&gt;Affinity не опустится ниже 40 единиц.&lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t>argoUpgrade_trainingModule3.Description.Name</t>
@@ -920,14 +920,14 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;b&gt;&lt;color=#F79232&gt;Allows you to Drop an Additional Vehicle&lt;/color&gt;&lt;/b&gt; 
-The Command and Control systems were never really intended to support a Light Company’s worth of ‘Mechs, Commander. If we want to maintain communications with our pilots, we’ll need to upgrade our communication networks to deal with the additional bandwidth.
+  The Command and Control systems were never really intended to support a Light Company’s worth of ‘Mechs, Commander. If we want to maintain communications with our pilots, we’ll need to upgrade our communication networks to deal with the additional bandwidth.
 ---
 &lt;b&gt;&lt;color=#F79232&gt;Allows you to Drop an Additional Vehicle&lt;/color&gt;&lt;/b&gt; 
  The Command and Control systems were never really intended to support a Light Company’s worth of ‘Mechs, Commander. If we want to maintain communications with our pilots, we’ll need to upgrade our communication networks to deal with the additional bandwidth.</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;b&gt;&lt;color=#F79232&gt;Позволяет высаживать дополнительную единицу техники.&lt;/color&gt;&lt;/b&gt; 
-Командир, системы управления и контроля никогда не предназначались для поддержки малобюджетных кампаний, у которых на вооружении лишь танки и лёгкие мехи. Если мы хотим поддерживать связь с нашими пилотами, нам нужно улучшить пропускную способность наших коммуникационных сетей.</t>
+  Командир, системы управления и контроля никогда не предназначались для поддержки малобюджетных кампаний, у которых на вооружении лишь танки и лёгкие мехи. Если мы хотим поддерживать связь с нашими пилотами, нам нужно улучшить пропускную способность наших коммуникационных сетей.</t>
   </si>
   <si>
     <t>argoUpgrade_VehicleSlot.Description.Name</t>
@@ -943,14 +943,14 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;b&gt;&lt;color=#F79232&gt;Allows you to Drop an Additional Vehicle&lt;/color&gt;&lt;/b&gt; 
-The upgrades continue commander. Interfacing this Star League technology with our own C&amp;C systems is proving challenging, but there's no problem more money and time can't fix, right?
+  The upgrades continue commander. Interfacing this Star League technology with our own C&amp;C systems is proving challenging, but there's no problem more money and time can't fix, right?
 ---
 &lt;b&gt;&lt;color=#F79232&gt;Allows you to Drop an Additional Vehicle&lt;/color&gt;&lt;/b&gt; 
  The upgrades continue commander. Interfacing this Star League technology with our own C&amp;C systems is proving challenging, but there's no problem more money and time can't fix, right?</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;b&gt;&lt;color=#F79232&gt;Позволяет высаживать дополнительную единицу техники.&lt;/color&gt;&lt;/b&gt; 
-Модернизация продолжается, командир. Наладить взаимодействие между технологией Звёздной лиги и нашей системой управления и контроля будет сложной задачей, но нет таких проблем, которые бы не смогли решить время и деньги, верно?</t>
+  Модернизация продолжается, командир. Наладить взаимодействие между технологией Звёздной лиги и нашей системой управления и контроля будет сложной задачей, но нет таких проблем, которые бы не смогли решить время и деньги, верно?</t>
   </si>
   <si>
     <t>argoUpgrade_VehicleSlot1.Description.Name</t>
@@ -969,7 +969,7 @@
   </si>
   <si>
     <t xml:space="preserve">Шаттл бросили ржаветь на свалке, командир. Большинство деталей каркаса &lt;i&gt;«Леопарда»&lt;/i&gt; держатся на ржавчине и честном слове. Мои техи могут приступить к починке самых проблемных участков, но должен предупредить, что на полный ремонт уйдёт очень много времени. 
-&lt;b&gt;&lt;color=#F79232&gt;Увеличивает лимит тоннажа высадки на 50 тонн.&lt;/color&gt;&lt;/b&gt;</t>
+ &lt;b&gt;&lt;color=#F79232&gt;Увеличивает лимит тоннажа высадки на 50 тонн.&lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t>argoUpgrade_WeightLimit.Description.Name</t>
@@ -1048,7 +1048,7 @@
   </si>
   <si>
     <t xml:space="preserve">Теперь, когда двигатели и структура корабля восстановлены, следующим шагом будет откалибровать системы управления, чтобы они учитывали изменения в балансе и производительности после нашего ремонта . Нам нужно совершить серию орбитальных высадок для точного измерения характеристик управляемости, а затем внести изменения в бортовые системы управления полетом.
-&lt;b&gt;&lt;color=#F79232&gt;Увеличивает лимит тоннажа высадки на 50 тонн.&lt;/color&gt;&lt;/b&gt;</t>
+ &lt;b&gt;&lt;color=#F79232&gt;Увеличивает лимит тоннажа высадки на 50 тонн.&lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t>argoUpgrade_WeightLimit6.Description.Name</t>
@@ -1061,7 +1061,7 @@
   </si>
   <si>
     <t xml:space="preserve">Хорошая новость - мы почти на финишной прямой! Честно говоря, я никогда не думал, что мы продвинемся так далеко, босс. Я откладывал этот разговор до этого момента из-за хронического недостатка времени и денег, но хребет корабля погнут. Он погнулся либо во время со своей предыдущей службы, либо когда гнил на свалке. Нам придется полностью разобрать корабль до основания, чтобы починить его, зато потом он будет как новенький! 
-&lt;b&gt;&lt;color=#F79232&gt;Увеличивает лимит тоннажа высадки на 50 тонн.&lt;/color&gt;&lt;/b&gt;</t>
+ &lt;b&gt;&lt;color=#F79232&gt;Увеличивает лимит тоннажа высадки на 50 тонн.&lt;/color&gt;&lt;/b&gt;</t>
   </si>
   <si>
     <t>argoUpgrade_WeightLimit7.Description.Name</t>
@@ -1103,17 +1103,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="2" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="2" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="2" applyFill="1" borderId="0" applyBorder="1" xfId="0" quotePrefix="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1409,18 +1403,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G114"/>
+  <dimension ref="A1:H114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="27.7109375" customWidth="1" style="2"/>
     <col min="2" max="3" width="94.5703125" customWidth="1" style="2"/>
-    <col min="4" max="6" width="9.140625" customWidth="1" style="2"/>
-    <col min="7" max="16384" width="9.140625" customWidth="1" style="2"/>
+    <col min="4" max="7" width="9.140625" customWidth="1" style="2"/>
+    <col min="8" max="16384" width="9.140625" customWidth="1" style="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1478,33 +1472,35 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" s="4" customFormat="1">
-      <c r="A6" s="4" t="s">
+    <row r="6" s="3" customFormat="1">
+      <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" ht="90" s="4" customFormat="1">
-      <c r="A7" s="4" t="s">
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" s="3" customFormat="1">
+      <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="G7" s="4"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="H7" s="3"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
@@ -1517,19 +1513,20 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" ht="75" s="4" customFormat="1">
-      <c r="A9" s="4" t="s">
+    <row r="9" s="3" customFormat="1">
+      <c r="A9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="G9" s="4"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="H9" s="3"/>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
@@ -1542,19 +1539,20 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" ht="75" s="4" customFormat="1">
-      <c r="A11" s="4" t="s">
+    <row r="11" s="3" customFormat="1">
+      <c r="A11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="G11" s="4"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="H11" s="3"/>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
@@ -1567,19 +1565,20 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" ht="120" s="4" customFormat="1">
-      <c r="A13" s="4" t="s">
+    <row r="13" s="3" customFormat="1">
+      <c r="A13" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="G13" s="4"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="H13" s="3"/>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
@@ -1658,14 +1657,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" ht="75">
+    <row r="21">
       <c r="A21" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="2" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1724,19 +1723,20 @@
         <v>71</v>
       </c>
     </row>
-    <row r="27" s="4" customFormat="1">
-      <c r="A27" s="4" t="s">
+    <row r="27" s="3" customFormat="1">
+      <c r="A27" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="G27" s="4"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="H27" s="3"/>
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
@@ -1793,19 +1793,20 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" ht="75" s="4" customFormat="1">
-      <c r="A33" s="4" t="s">
+    <row r="33" s="3" customFormat="1">
+      <c r="A33" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="G33" s="4"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="H33" s="3"/>
     </row>
     <row r="34">
       <c r="A34" s="2" t="s">
@@ -1818,19 +1819,20 @@
         <v>95</v>
       </c>
     </row>
-    <row r="35" ht="90" s="4" customFormat="1">
-      <c r="A35" s="4" t="s">
+    <row r="35" s="3" customFormat="1">
+      <c r="A35" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="G35" s="4"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="H35" s="3"/>
     </row>
     <row r="36">
       <c r="A36" s="2" t="s">
@@ -1953,19 +1955,20 @@
         <v>131</v>
       </c>
     </row>
-    <row r="47" ht="90" s="4" customFormat="1">
-      <c r="A47" s="4" t="s">
+    <row r="47" s="3" customFormat="1">
+      <c r="A47" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="C47" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
-      <c r="G47" s="4"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="H47" s="3"/>
     </row>
     <row r="48">
       <c r="A48" s="2" t="s">
@@ -1978,19 +1981,20 @@
         <v>137</v>
       </c>
     </row>
-    <row r="49" ht="60" s="4" customFormat="1">
-      <c r="A49" s="4" t="s">
+    <row r="49" s="3" customFormat="1">
+      <c r="A49" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="C49" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
-      <c r="G49" s="4"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="H49" s="3"/>
     </row>
     <row r="50">
       <c r="A50" s="2" t="s">
@@ -2355,19 +2359,20 @@
         <v>239</v>
       </c>
     </row>
-    <row r="83" ht="120" s="4" customFormat="1">
-      <c r="A83" s="4" t="s">
+    <row r="83" s="3" customFormat="1">
+      <c r="A83" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="B83" s="5" t="s">
+      <c r="B83" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="C83" s="5" t="s">
+      <c r="C83" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="D83" s="4"/>
-      <c r="E83" s="4"/>
-      <c r="G83" s="4"/>
+      <c r="D83" s="3"/>
+      <c r="E83" s="3"/>
+      <c r="F83" s="3"/>
+      <c r="H83" s="3"/>
     </row>
     <row r="84">
       <c r="A84" s="2" t="s">
@@ -2380,19 +2385,20 @@
         <v>245</v>
       </c>
     </row>
-    <row r="85" ht="105" s="4" customFormat="1">
-      <c r="A85" s="4" t="s">
+    <row r="85" s="3" customFormat="1">
+      <c r="A85" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="B85" s="5" t="s">
+      <c r="B85" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="C85" s="5" t="s">
+      <c r="C85" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="D85" s="4"/>
-      <c r="E85" s="4"/>
-      <c r="G85" s="4"/>
+      <c r="D85" s="3"/>
+      <c r="E85" s="3"/>
+      <c r="F85" s="3"/>
+      <c r="H85" s="3"/>
     </row>
     <row r="86">
       <c r="A86" s="2" t="s">
@@ -2405,19 +2411,20 @@
         <v>245</v>
       </c>
     </row>
-    <row r="87" ht="120" s="4" customFormat="1">
-      <c r="A87" s="4" t="s">
+    <row r="87" s="3" customFormat="1">
+      <c r="A87" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="B87" s="5" t="s">
+      <c r="B87" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="C87" s="5" t="s">
+      <c r="C87" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="D87" s="4"/>
-      <c r="E87" s="4"/>
-      <c r="G87" s="4"/>
+      <c r="D87" s="3"/>
+      <c r="E87" s="3"/>
+      <c r="F87" s="3"/>
+      <c r="H87" s="3"/>
     </row>
     <row r="88">
       <c r="A88" s="2" t="s">
@@ -2430,19 +2437,20 @@
         <v>245</v>
       </c>
     </row>
-    <row r="89" ht="105" s="4" customFormat="1">
-      <c r="A89" s="4" t="s">
+    <row r="89" s="3" customFormat="1">
+      <c r="A89" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="B89" s="5" t="s">
+      <c r="B89" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="C89" s="5" t="s">
+      <c r="C89" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="D89" s="4"/>
-      <c r="E89" s="4"/>
-      <c r="G89" s="4"/>
+      <c r="D89" s="3"/>
+      <c r="E89" s="3"/>
+      <c r="F89" s="3"/>
+      <c r="H89" s="3"/>
     </row>
     <row r="90">
       <c r="A90" s="2" t="s">
@@ -2455,19 +2463,20 @@
         <v>259</v>
       </c>
     </row>
-    <row r="91" ht="120" s="4" customFormat="1">
-      <c r="A91" s="4" t="s">
+    <row r="91" s="3" customFormat="1">
+      <c r="A91" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="B91" s="5" t="s">
+      <c r="B91" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="C91" s="5" t="s">
+      <c r="C91" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="D91" s="4"/>
-      <c r="E91" s="4"/>
-      <c r="G91" s="4"/>
+      <c r="D91" s="3"/>
+      <c r="E91" s="3"/>
+      <c r="F91" s="3"/>
+      <c r="H91" s="3"/>
     </row>
     <row r="92">
       <c r="A92" s="2" t="s">
@@ -2480,19 +2489,20 @@
         <v>265</v>
       </c>
     </row>
-    <row r="93" ht="120" s="4" customFormat="1">
-      <c r="A93" s="4" t="s">
+    <row r="93" s="3" customFormat="1">
+      <c r="A93" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="B93" s="5" t="s">
+      <c r="B93" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="C93" s="5" t="s">
+      <c r="C93" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="D93" s="4"/>
-      <c r="E93" s="4"/>
-      <c r="G93" s="4"/>
+      <c r="D93" s="3"/>
+      <c r="E93" s="3"/>
+      <c r="F93" s="3"/>
+      <c r="H93" s="3"/>
     </row>
     <row r="94">
       <c r="A94" s="2" t="s">
@@ -2505,19 +2515,20 @@
         <v>271</v>
       </c>
     </row>
-    <row r="95" ht="90" s="4" customFormat="1">
-      <c r="A95" s="4" t="s">
+    <row r="95" s="3" customFormat="1">
+      <c r="A95" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="B95" s="5" t="s">
+      <c r="B95" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="C95" s="5" t="s">
+      <c r="C95" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="D95" s="4"/>
-      <c r="E95" s="4"/>
-      <c r="G95" s="4"/>
+      <c r="D95" s="3"/>
+      <c r="E95" s="3"/>
+      <c r="F95" s="3"/>
+      <c r="H95" s="3"/>
     </row>
     <row r="96">
       <c r="A96" s="2" t="s">
@@ -2530,19 +2541,20 @@
         <v>277</v>
       </c>
     </row>
-    <row r="97" ht="75" s="4" customFormat="1">
-      <c r="A97" s="4" t="s">
+    <row r="97" s="3" customFormat="1">
+      <c r="A97" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="B97" s="5" t="s">
+      <c r="B97" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="C97" s="5" t="s">
+      <c r="C97" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="D97" s="4"/>
-      <c r="E97" s="4"/>
-      <c r="G97" s="4"/>
+      <c r="D97" s="3"/>
+      <c r="E97" s="3"/>
+      <c r="F97" s="3"/>
+      <c r="H97" s="3"/>
     </row>
     <row r="98">
       <c r="A98" s="2" t="s">
@@ -2555,14 +2567,14 @@
         <v>283</v>
       </c>
     </row>
-    <row r="99" ht="60">
+    <row r="99">
       <c r="A99" s="2" t="s">
         <v>284</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="C99" s="3" t="s">
+      <c r="C99" s="2" t="s">
         <v>286</v>
       </c>
     </row>
@@ -2687,14 +2699,14 @@
         <v>289</v>
       </c>
     </row>
-    <row r="111" ht="90">
+    <row r="111">
       <c r="A111" s="2" t="s">
         <v>310</v>
       </c>
       <c r="B111" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="C111" s="3" t="s">
+      <c r="C111" s="2" t="s">
         <v>312</v>
       </c>
     </row>
@@ -2709,14 +2721,14 @@
         <v>289</v>
       </c>
     </row>
-    <row r="113" ht="90">
+    <row r="113">
       <c r="A113" s="2" t="s">
         <v>314</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="C113" s="3" t="s">
+      <c r="C113" s="2" t="s">
         <v>316</v>
       </c>
     </row>

</xml_diff>